<commit_message>
optimised mvp temp, cleaned up
</commit_message>
<xml_diff>
--- a/data/templates/multimarketplace_mvp_template.xlsx
+++ b/data/templates/multimarketplace_mvp_template.xlsx
@@ -29,7 +29,7 @@
       <b val="1"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill/>
     </fill>
@@ -40,6 +40,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="00FFE6E6"/>
         <bgColor rgb="00FFE6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00E6FFE6"/>
+        <bgColor rgb="00E6FFE6"/>
       </patternFill>
     </fill>
   </fills>
@@ -61,9 +67,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -431,7 +440,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:AP1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -445,6 +454,42 @@
     <col width="60" customWidth="1" min="4" max="4"/>
     <col width="20" customWidth="1" min="5" max="5"/>
     <col width="15" customWidth="1" min="6" max="6"/>
+    <col width="15" customWidth="1" min="7" max="7"/>
+    <col width="15" customWidth="1" min="8" max="8"/>
+    <col width="20" customWidth="1" min="9" max="9"/>
+    <col width="20" customWidth="1" min="10" max="10"/>
+    <col width="20" customWidth="1" min="11" max="11"/>
+    <col width="15" customWidth="1" min="12" max="12"/>
+    <col width="15" customWidth="1" min="13" max="13"/>
+    <col width="15" customWidth="1" min="14" max="14"/>
+    <col width="25" customWidth="1" min="15" max="15"/>
+    <col width="20" customWidth="1" min="16" max="16"/>
+    <col width="40" customWidth="1" min="17" max="17"/>
+    <col width="40" customWidth="1" min="18" max="18"/>
+    <col width="60" customWidth="1" min="19" max="19"/>
+    <col width="60" customWidth="1" min="20" max="20"/>
+    <col width="20" customWidth="1" min="21" max="21"/>
+    <col width="30" customWidth="1" min="22" max="22"/>
+    <col width="30" customWidth="1" min="23" max="23"/>
+    <col width="30" customWidth="1" min="24" max="24"/>
+    <col width="30" customWidth="1" min="25" max="25"/>
+    <col width="30" customWidth="1" min="26" max="26"/>
+    <col width="30" customWidth="1" min="27" max="27"/>
+    <col width="20" customWidth="1" min="28" max="28"/>
+    <col width="40" customWidth="1" min="29" max="29"/>
+    <col width="60" customWidth="1" min="30" max="30"/>
+    <col width="30" customWidth="1" min="31" max="31"/>
+    <col width="30" customWidth="1" min="32" max="32"/>
+    <col width="30" customWidth="1" min="33" max="33"/>
+    <col width="40" customWidth="1" min="34" max="34"/>
+    <col width="40" customWidth="1" min="35" max="35"/>
+    <col width="40" customWidth="1" min="36" max="36"/>
+    <col width="40" customWidth="1" min="37" max="37"/>
+    <col width="60" customWidth="1" min="38" max="38"/>
+    <col width="60" customWidth="1" min="39" max="39"/>
+    <col width="60" customWidth="1" min="40" max="40"/>
+    <col width="60" customWidth="1" min="41" max="41"/>
+    <col width="15" customWidth="1" min="42" max="42"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -476,6 +521,186 @@
       <c r="F1" s="1" t="inlineStr">
         <is>
           <t>Brand</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Pack quantity</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Pack type</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>Product type</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>Product thickness (mm)</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>Product width (mm)</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>Colour group</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>Effect</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>Location</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>Facet_product_type</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>Seller Product ID</t>
+        </is>
+      </c>
+      <c r="Q1" s="2" t="inlineStr">
+        <is>
+          <t>Product Title (nl_BE)</t>
+        </is>
+      </c>
+      <c r="R1" s="2" t="inlineStr">
+        <is>
+          <t>Product Title (fr_BE)</t>
+        </is>
+      </c>
+      <c r="S1" s="2" t="inlineStr">
+        <is>
+          <t>Description (nl_BE)</t>
+        </is>
+      </c>
+      <c r="T1" s="2" t="inlineStr">
+        <is>
+          <t>Description (fr_BE)</t>
+        </is>
+      </c>
+      <c r="U1" s="1" t="inlineStr">
+        <is>
+          <t>Image 2</t>
+        </is>
+      </c>
+      <c r="V1" s="2" t="inlineStr">
+        <is>
+          <t>USP 1 nl_be</t>
+        </is>
+      </c>
+      <c r="W1" s="2" t="inlineStr">
+        <is>
+          <t>USP 2 nl_be</t>
+        </is>
+      </c>
+      <c r="X1" s="2" t="inlineStr">
+        <is>
+          <t>USP 3 nl_be</t>
+        </is>
+      </c>
+      <c r="Y1" s="2" t="inlineStr">
+        <is>
+          <t>USP 1 fr_be</t>
+        </is>
+      </c>
+      <c r="Z1" s="2" t="inlineStr">
+        <is>
+          <t>USP 2 fr_be</t>
+        </is>
+      </c>
+      <c r="AA1" s="2" t="inlineStr">
+        <is>
+          <t>USP 3 fr_be</t>
+        </is>
+      </c>
+      <c r="AB1" s="1" t="inlineStr">
+        <is>
+          <t>Material</t>
+        </is>
+      </c>
+      <c r="AC1" s="2" t="inlineStr">
+        <is>
+          <t>Product Title (nl_NL)</t>
+        </is>
+      </c>
+      <c r="AD1" s="2" t="inlineStr">
+        <is>
+          <t>Description (nl_NL)</t>
+        </is>
+      </c>
+      <c r="AE1" s="2" t="inlineStr">
+        <is>
+          <t>USP 1 (nl_NL)</t>
+        </is>
+      </c>
+      <c r="AF1" s="2" t="inlineStr">
+        <is>
+          <t>USP 2 (nl_NL)</t>
+        </is>
+      </c>
+      <c r="AG1" s="2" t="inlineStr">
+        <is>
+          <t>USP 3 (nl_NL)</t>
+        </is>
+      </c>
+      <c r="AH1" s="2" t="inlineStr">
+        <is>
+          <t>Product Title FR</t>
+        </is>
+      </c>
+      <c r="AI1" s="2" t="inlineStr">
+        <is>
+          <t>Product Title IT</t>
+        </is>
+      </c>
+      <c r="AJ1" s="2" t="inlineStr">
+        <is>
+          <t>Product Title ES</t>
+        </is>
+      </c>
+      <c r="AK1" s="2" t="inlineStr">
+        <is>
+          <t>Product Title PT</t>
+        </is>
+      </c>
+      <c r="AL1" s="2" t="inlineStr">
+        <is>
+          <t>Long Description FR</t>
+        </is>
+      </c>
+      <c r="AM1" s="2" t="inlineStr">
+        <is>
+          <t>Long Description IT</t>
+        </is>
+      </c>
+      <c r="AN1" s="2" t="inlineStr">
+        <is>
+          <t>Long Description ES</t>
+        </is>
+      </c>
+      <c r="AO1" s="2" t="inlineStr">
+        <is>
+          <t>Long Description PT</t>
+        </is>
+      </c>
+      <c r="AP1" s="1" t="inlineStr">
+        <is>
+          <t>Contains wood</t>
         </is>
       </c>
     </row>

</xml_diff>